<commit_message>
1mer commit desde desktop/clon
</commit_message>
<xml_diff>
--- a/exquesisepuede.xlsx
+++ b/exquesisepuede.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TERRY\Desktop\Prueba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TERRY\Desktop\probandosubirdocexc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F37801-F521-4989-8E34-8EFE1FD8B40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87A0710-ECE4-4B4E-94EE-CC6D821DB0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>sd</t>
   </si>
   <si>
     <t>ds</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -348,27 +354,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>